<commit_message>
Dodati zadaci i konvencija
</commit_message>
<xml_diff>
--- a/Sprint_info/Sprint1.xlsx
+++ b/Sprint_info/Sprint1.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nevidjen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nevidjen\Documents\GitHub\MasterAudioTechnologyFunctions\Sprint_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Rooster" sheetId="2" r:id="rId1"/>
+    <sheet name="Roster" sheetId="2" r:id="rId1"/>
     <sheet name="Sprint" sheetId="1" r:id="rId2"/>
     <sheet name="Chart" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
-  <si>
-    <t>Team rooster</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -52,9 +49,6 @@
     <t>Vanja Cvetković</t>
   </si>
   <si>
-    <t>Developer</t>
-  </si>
-  <si>
     <t>1126/2015</t>
   </si>
   <si>
@@ -143,6 +137,45 @@
   </si>
   <si>
     <t>Actually left</t>
+  </si>
+  <si>
+    <t>Team roster</t>
+  </si>
+  <si>
+    <t>Lead developer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Playing music and flow control </t>
+  </si>
+  <si>
+    <t>Find library that implements play functionality</t>
+  </si>
+  <si>
+    <t>Implement play functionality</t>
+  </si>
+  <si>
+    <t>Review code</t>
+  </si>
+  <si>
+    <t>Document implementation</t>
+  </si>
+  <si>
+    <t>Implement basic GUI</t>
+  </si>
+  <si>
+    <t>Create flow controls and buttons</t>
+  </si>
+  <si>
+    <t>Implement file chooser</t>
+  </si>
+  <si>
+    <t>Timeline</t>
+  </si>
+  <si>
+    <t>To do</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -152,7 +185,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,7 +230,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -327,19 +360,6 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top/>
       <bottom style="thin">
@@ -393,12 +413,11 @@
     <xf numFmtId="14" fontId="2" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -408,35 +427,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="40% Akcenat3" xfId="1" builtinId="39"/>
-    <cellStyle name="Akcenat6" xfId="2" builtinId="49"/>
-    <cellStyle name="Normalan" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent3" xfId="1" builtinId="39"/>
+    <cellStyle name="Accent6" xfId="2" builtinId="49"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -554,7 +576,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="sr-Latn-RS"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -569,7 +591,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sprint!$E$12</c:f>
+              <c:f>Sprint!$E$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -648,54 +670,54 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sprint!$F$12:$T$12</c:f>
+              <c:f>Sprint!$F$15:$T$15</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>26.928571428571427</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>24.857142857142854</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>22.785714285714281</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>20.714285714285708</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>18.642857142857135</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>16.571428571428562</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>14.499999999999991</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>12.42857142857142</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>10.357142857142849</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>8.2857142857142776</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>6.2142857142857064</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>4.1428571428571352</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>2.0714285714285636</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>-7.9936057773011271E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -712,7 +734,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sprint!$E$13</c:f>
+              <c:f>Sprint!$E$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -791,54 +813,54 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sprint!$F$13:$T$13</c:f>
+              <c:f>Sprint!$F$16:$T$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -926,7 +948,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="sr-Latn-RS"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -963,7 +985,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="308624616"/>
@@ -1043,7 +1065,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="sr-Latn-RS"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1074,7 +1096,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="sr-Latn-RS"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="308619040"/>
@@ -1125,7 +1147,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="sr-Latn-RS"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1173,7 +1195,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="sr-Latn-RS"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2063,69 +2085,69 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="26"/>
+      <c r="B2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="14" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="15" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>3</v>
       </c>
+      <c r="B3" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="16" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="22" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="17" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="22" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="17" t="s">
+      <c r="B5" s="22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="5" t="s">
+      <c r="C5" s="22"/>
+      <c r="D5" s="17" t="s">
         <v>10</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="18" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2142,116 +2164,129 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="15" width="5.7109375" customWidth="1"/>
     <col min="16" max="19" width="6.7109375" customWidth="1"/>
-    <col min="20" max="20" width="8.7109375" customWidth="1"/>
+    <col min="20" max="20" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="7">
-        <v>42432</v>
+        <v>42434</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="9">
+        <f>C1+14</f>
+        <v>42448</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="9">
-        <v>42446</v>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
-      <c r="A4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="26">
+        <v>13</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -2268,16 +2303,24 @@
       <c r="T5" s="2"/>
       <c r="U5" s="2">
         <f>E5-SUM(G5:T5)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="26"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -2293,17 +2336,25 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
       <c r="U6" s="2">
-        <f t="shared" ref="U6:U11" si="0">E6-SUM(G6:T6)</f>
-        <v>0</v>
+        <f t="shared" ref="U6:U14" si="0">E6-SUM(G6:T6)</f>
+        <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -2319,17 +2370,25 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>E7-SUM(G7:T7)</f>
+        <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
-      <c r="A8" s="27"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>3</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -2346,16 +2405,28 @@
       <c r="T8" s="2"/>
       <c r="U8" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
-      <c r="A9" s="27"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="27">
+        <v>8</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -2372,16 +2443,24 @@
       <c r="T9" s="2"/>
       <c r="U9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
-      <c r="A10" s="27"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="26"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -2398,263 +2477,367 @@
       <c r="T10" s="2"/>
       <c r="U10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
-      <c r="A11" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="11">
-        <f>SUM(B5:B10)</f>
-        <v>0</v>
-      </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11">
-        <f>SUM(E5:E10)</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11">
-        <f>SUM(G5:G10)</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="11">
-        <f>SUM(H5:H10)</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="11">
-        <f t="shared" ref="I11:T11" si="1">SUM(I5:I10)</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K11" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L11" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M11" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N11" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P11" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q11" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="R11" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S11" s="11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="T11" s="12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="26"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
       <c r="U11" s="2">
         <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="26"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="26"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="2">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2">
+        <f>SUM(B5:B13)</f>
+        <v>21</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="2">
+        <f>SUM(E5:E13)</f>
+        <v>29</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" s="2">
+        <f>SUM(G5:G13)</f>
         <v>0</v>
       </c>
+      <c r="H14" s="2">
+        <f>SUM(H5:H13)</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <f>SUM(I5:I13)</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <f>SUM(J5:J13)</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <f>SUM(K5:K13)</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
+        <f>SUM(L5:L13)</f>
+        <v>0</v>
+      </c>
+      <c r="M14" s="2">
+        <f>SUM(M5:M13)</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="2">
+        <f>SUM(N5:N13)</f>
+        <v>0</v>
+      </c>
+      <c r="O14" s="2">
+        <f>SUM(O5:O13)</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="2">
+        <f>SUM(P5:P13)</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="2">
+        <f>SUM(Q5:Q13)</f>
+        <v>0</v>
+      </c>
+      <c r="R14" s="2">
+        <f>SUM(R5:R13)</f>
+        <v>0</v>
+      </c>
+      <c r="S14" s="2">
+        <f>SUM(S5:S13)</f>
+        <v>0</v>
+      </c>
+      <c r="T14" s="2">
+        <f>SUM(T5:T13)</f>
+        <v>0</v>
+      </c>
+      <c r="U14" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
     </row>
-    <row r="12" spans="1:21">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="2">
-        <f>SUM(E5:E10)</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="20">
-        <f>F12-F12/14</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="20">
-        <f>G12-F12/14</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="20">
-        <f>H12-F12/14</f>
-        <v>0</v>
-      </c>
-      <c r="J12" s="20">
-        <f>I12-F12/14</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="20">
-        <f>J12-F12/14</f>
-        <v>0</v>
-      </c>
-      <c r="L12" s="20">
-        <f>K12-F12/14</f>
-        <v>0</v>
-      </c>
-      <c r="M12" s="20">
-        <f>L12-F12/14</f>
-        <v>0</v>
-      </c>
-      <c r="N12" s="20">
-        <f>M12-F12/14</f>
-        <v>0</v>
-      </c>
-      <c r="O12" s="20">
-        <f>N12-F12/14</f>
-        <v>0</v>
-      </c>
-      <c r="P12" s="20">
-        <f>O12-F12/14</f>
-        <v>0</v>
-      </c>
-      <c r="Q12" s="20">
-        <f>P12-F12/14</f>
-        <v>0</v>
-      </c>
-      <c r="R12" s="20">
-        <f>Q12-F12/14</f>
-        <v>0</v>
-      </c>
-      <c r="S12" s="20">
-        <f>R12-F12/14</f>
-        <v>0</v>
-      </c>
-      <c r="T12" s="20">
-        <f>S12-F12/14</f>
-        <v>0</v>
-      </c>
-      <c r="U12" s="13"/>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="2">
+        <f>SUM(E5:E13)</f>
+        <v>29</v>
+      </c>
+      <c r="G15" s="19">
+        <f>F15-F15/14</f>
+        <v>26.928571428571427</v>
+      </c>
+      <c r="H15" s="19">
+        <f>G15-F15/14</f>
+        <v>24.857142857142854</v>
+      </c>
+      <c r="I15" s="19">
+        <f>H15-F15/14</f>
+        <v>22.785714285714281</v>
+      </c>
+      <c r="J15" s="19">
+        <f>I15-F15/14</f>
+        <v>20.714285714285708</v>
+      </c>
+      <c r="K15" s="19">
+        <f>J15-F15/14</f>
+        <v>18.642857142857135</v>
+      </c>
+      <c r="L15" s="19">
+        <f>K15-F15/14</f>
+        <v>16.571428571428562</v>
+      </c>
+      <c r="M15" s="19">
+        <f>L15-F15/14</f>
+        <v>14.499999999999991</v>
+      </c>
+      <c r="N15" s="19">
+        <f>M15-F15/14</f>
+        <v>12.42857142857142</v>
+      </c>
+      <c r="O15" s="19">
+        <f>N15-F15/14</f>
+        <v>10.357142857142849</v>
+      </c>
+      <c r="P15" s="19">
+        <f>O15-F15/14</f>
+        <v>8.2857142857142776</v>
+      </c>
+      <c r="Q15" s="19">
+        <f>P15-F15/14</f>
+        <v>6.2142857142857064</v>
+      </c>
+      <c r="R15" s="19">
+        <f>Q15-F15/14</f>
+        <v>4.1428571428571352</v>
+      </c>
+      <c r="S15" s="19">
+        <f>R15-F15/14</f>
+        <v>2.0714285714285636</v>
+      </c>
+      <c r="T15" s="19">
+        <f>S15-F15/14</f>
+        <v>-7.9936057773011271E-15</v>
+      </c>
+      <c r="U15" s="12"/>
     </row>
-    <row r="13" spans="1:21">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="2">
-        <f>SUM(E5:E10)</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="2">
-        <f>F13-SUM(G5:G10)</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="2">
-        <f t="shared" ref="H13:T13" si="2">G13-SUM(H5:H10)</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L13" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="N13" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P13" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R13" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="S13" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T13" s="2">
-        <f>S13-SUM(T5:T10)</f>
-        <v>0</v>
-      </c>
-      <c r="U13" s="13"/>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="2">
+        <f>SUM(E5:E13)</f>
+        <v>29</v>
+      </c>
+      <c r="G16" s="2">
+        <f>F16-SUM(G5:G13)</f>
+        <v>29</v>
+      </c>
+      <c r="H16" s="2">
+        <f>G16-SUM(H5:H13)</f>
+        <v>29</v>
+      </c>
+      <c r="I16" s="2">
+        <f>H16-SUM(I5:I13)</f>
+        <v>29</v>
+      </c>
+      <c r="J16" s="2">
+        <f>I16-SUM(J5:J13)</f>
+        <v>29</v>
+      </c>
+      <c r="K16" s="2">
+        <f>J16-SUM(K5:K13)</f>
+        <v>29</v>
+      </c>
+      <c r="L16" s="2">
+        <f>K16-SUM(L5:L13)</f>
+        <v>29</v>
+      </c>
+      <c r="M16" s="2">
+        <f>L16-SUM(M5:M13)</f>
+        <v>29</v>
+      </c>
+      <c r="N16" s="2">
+        <f>M16-SUM(N5:N13)</f>
+        <v>29</v>
+      </c>
+      <c r="O16" s="2">
+        <f>N16-SUM(O5:O13)</f>
+        <v>29</v>
+      </c>
+      <c r="P16" s="2">
+        <f>O16-SUM(P5:P13)</f>
+        <v>29</v>
+      </c>
+      <c r="Q16" s="2">
+        <f>P16-SUM(Q5:Q13)</f>
+        <v>29</v>
+      </c>
+      <c r="R16" s="2">
+        <f>Q16-SUM(R5:R13)</f>
+        <v>29</v>
+      </c>
+      <c r="S16" s="2">
+        <f>R16-SUM(S5:S13)</f>
+        <v>29</v>
+      </c>
+      <c r="T16" s="2">
+        <f>S16-SUM(T5:T13)</f>
+        <v>29</v>
+      </c>
+      <c r="U16" s="12"/>
     </row>
-    <row r="15" spans="1:21">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
     </row>
-    <row r="16" spans="1:21">
-      <c r="A16" s="13"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="13"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="12"/>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="13"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="13"/>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="12"/>
     </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="13"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="13"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="12"/>
     </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="13"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="13"/>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="B9:B13"/>
   </mergeCells>
-  <conditionalFormatting sqref="F5:F10">
+  <conditionalFormatting sqref="F5:F14">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
@@ -2665,13 +2848,13 @@
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U5:U11">
+  <conditionalFormatting sqref="U5:U14">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="491" yWindow="329" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F14">
       <formula1>"To do, In progress, Done"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2682,9 +2865,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="491" yWindow="329" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a valid name" promptTitle="Names" prompt="Enter assignee">
           <x14:formula1>
-            <xm:f>Rooster!$A$3:$A$5</xm:f>
+            <xm:f>Roster!$A$3:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D10</xm:sqref>
+          <xm:sqref>D5:D13</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2696,11 +2879,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Sprint1 daily scrum meeting day3
</commit_message>
<xml_diff>
--- a/Sprint_info/Sprint1.xlsx
+++ b/Sprint_info/Sprint1.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="2" r:id="rId1"/>
     <sheet name="Sprint" sheetId="1" r:id="rId2"/>
     <sheet name="Chart" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171026"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>To do</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -427,6 +433,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -457,8 +465,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="3" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent3" xfId="1" builtinId="39"/>
@@ -827,46 +833,46 @@
                   <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>29</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2101,21 +2107,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="22"/>
       <c r="D2" s="13" t="s">
         <v>2</v>
       </c>
@@ -2124,10 +2130,10 @@
       <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="21"/>
+      <c r="C3" s="23"/>
       <c r="D3" s="15" t="s">
         <v>7</v>
       </c>
@@ -2136,10 +2142,10 @@
       <c r="A4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="21"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="15" t="s">
         <v>5</v>
       </c>
@@ -2148,10 +2154,10 @@
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="16" t="s">
         <v>10</v>
       </c>
@@ -2172,8 +2178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2275,10 +2281,10 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="28">
         <v>13</v>
       </c>
       <c r="C5" s="19" t="s">
@@ -2291,11 +2297,13 @@
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="I5" s="2">
+        <v>2</v>
+      </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -2309,12 +2317,12 @@
       <c r="T5" s="2"/>
       <c r="U5" s="2">
         <f>E5-SUM(G5:T5)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
-      <c r="B6" s="26"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="19" t="s">
         <v>41</v>
       </c>
@@ -2325,7 +2333,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -2347,8 +2355,8 @@
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="19" t="s">
         <v>42</v>
       </c>
@@ -2381,8 +2389,8 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="19" t="s">
         <v>43</v>
       </c>
@@ -2415,10 +2423,10 @@
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="29">
         <v>8</v>
       </c>
       <c r="C9" s="19" t="s">
@@ -2431,9 +2439,11 @@
         <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G9" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -2449,12 +2459,12 @@
       <c r="T9" s="2"/>
       <c r="U9" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="28"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="19" t="s">
         <v>46</v>
       </c>
@@ -2487,8 +2497,8 @@
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="28"/>
+      <c r="A11" s="28"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="19" t="s">
         <v>47</v>
       </c>
@@ -2521,8 +2531,8 @@
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="28"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="19" t="s">
         <v>42</v>
       </c>
@@ -2555,8 +2565,8 @@
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="29"/>
+      <c r="A13" s="28"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="19" t="s">
         <v>43</v>
       </c>
@@ -2596,16 +2606,16 @@
         <f>SUM(B5:B13)</f>
         <v>21</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
       <c r="E14" s="2">
         <f>SUM(E5:E13)</f>
         <v>29</v>
       </c>
-      <c r="F14" s="30"/>
+      <c r="F14" s="20"/>
       <c r="G14" s="2">
         <f t="shared" ref="G14:T14" si="1">SUM(G5:G13)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="1"/>
@@ -2613,7 +2623,7 @@
       </c>
       <c r="I14" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" si="1"/>
@@ -2661,7 +2671,7 @@
       </c>
       <c r="U14" s="2">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -2748,59 +2758,59 @@
       </c>
       <c r="G16" s="2">
         <f t="shared" ref="G16:T16" si="2">F16-SUM(G5:G13)</f>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L16" s="2">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M16" s="2">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="N16" s="2">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="O16" s="2">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="P16" s="2">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="Q16" s="2">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="R16" s="2">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="S16" s="2">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="T16" s="2">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="U16" s="11"/>
     </row>
@@ -2883,7 +2893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Sprint1 daily scrum meeting day 4
</commit_message>
<xml_diff>
--- a/Sprint_info/Sprint1.xlsx
+++ b/Sprint_info/Sprint1.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="2" r:id="rId1"/>
     <sheet name="Sprint" sheetId="1" r:id="rId2"/>
     <sheet name="Chart" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2178,8 +2178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2475,7 +2475,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -2893,7 +2893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Sprint1 daily scrum meetings day 5 and 6
</commit_message>
<xml_diff>
--- a/Sprint_info/Sprint1.xlsx
+++ b/Sprint_info/Sprint1.xlsx
@@ -842,37 +842,37 @@
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>26</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>26</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>26</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>26</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>26</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>26</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2179,7 +2179,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2439,14 +2439,16 @@
         <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G9" s="2">
         <v>1</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="J9" s="2">
+        <v>1</v>
+      </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -2459,7 +2461,7 @@
       <c r="T9" s="2"/>
       <c r="U9" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -2475,12 +2477,14 @@
         <v>2</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="J10" s="2">
+        <v>2</v>
+      </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
@@ -2493,7 +2497,7 @@
       <c r="T10" s="2"/>
       <c r="U10" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -2509,7 +2513,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -2543,7 +2547,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -2627,7 +2631,7 @@
       </c>
       <c r="J14" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K14" s="2">
         <f t="shared" si="1"/>
@@ -2671,7 +2675,7 @@
       </c>
       <c r="U14" s="2">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -2770,47 +2774,47 @@
       </c>
       <c r="J16" s="2">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K16" s="2">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L16" s="2">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="M16" s="2">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="N16" s="2">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="O16" s="2">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="P16" s="2">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="Q16" s="2">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="R16" s="2">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="S16" s="2">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="T16" s="2">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="U16" s="11"/>
     </row>

</xml_diff>

<commit_message>
Sprint1 daily scrum meeting day 7, 8 and 9
</commit_message>
<xml_diff>
--- a/Sprint_info/Sprint1.xlsx
+++ b/Sprint_info/Sprint1.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sprint" sheetId="1" r:id="rId2"/>
     <sheet name="Chart" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -851,28 +851,28 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>23</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>23</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2178,8 +2178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2333,7 +2333,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -2341,8 +2341,12 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
+      <c r="M6" s="2">
+        <v>4</v>
+      </c>
+      <c r="N6" s="2">
+        <v>4</v>
+      </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
@@ -2351,7 +2355,7 @@
       <c r="T6" s="2"/>
       <c r="U6" s="2">
         <f t="shared" ref="U6:U14" si="0">E6-SUM(G6:T6)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -2367,7 +2371,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -2377,7 +2381,9 @@
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
+      <c r="O7" s="2">
+        <v>1</v>
+      </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
@@ -2385,7 +2391,7 @@
       <c r="T7" s="2"/>
       <c r="U7" s="2">
         <f>E7-SUM(G7:T7)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -2401,7 +2407,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -2557,7 +2563,9 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
+      <c r="O12" s="2">
+        <v>1</v>
+      </c>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
@@ -2565,7 +2573,7 @@
       <c r="T12" s="2"/>
       <c r="U12" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -2643,15 +2651,15 @@
       </c>
       <c r="M14" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N14" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O14" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P14" s="2">
         <f t="shared" si="1"/>
@@ -2675,7 +2683,7 @@
       </c>
       <c r="U14" s="2">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -2786,35 +2794,35 @@
       </c>
       <c r="M16" s="2">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="N16" s="2">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="O16" s="2">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="P16" s="2">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="Q16" s="2">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="R16" s="2">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="S16" s="2">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="T16" s="2">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="U16" s="11"/>
     </row>

</xml_diff>

<commit_message>
Sprint daily meeting day 10
</commit_message>
<xml_diff>
--- a/Sprint_info/Sprint1.xlsx
+++ b/Sprint_info/Sprint1.xlsx
@@ -860,19 +860,19 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2179,7 +2179,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2553,7 +2553,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -2566,14 +2566,16 @@
       <c r="O12" s="2">
         <v>1</v>
       </c>
-      <c r="P12" s="2"/>
+      <c r="P12" s="2">
+        <v>1</v>
+      </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -2663,7 +2665,7 @@
       </c>
       <c r="P14" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14" s="2">
         <f t="shared" si="1"/>
@@ -2683,7 +2685,7 @@
       </c>
       <c r="U14" s="2">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -2806,23 +2808,23 @@
       </c>
       <c r="P16" s="2">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q16" s="2">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R16" s="2">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S16" s="2">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T16" s="2">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U16" s="11"/>
     </row>

</xml_diff>

<commit_message>
Scrum daily meeting day 11  and 12
</commit_message>
<xml_diff>
--- a/Sprint_info/Sprint1.xlsx
+++ b/Sprint_info/Sprint1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -170,9 +170,6 @@
   </si>
   <si>
     <t>Timeline</t>
-  </si>
-  <si>
-    <t>To do</t>
   </si>
   <si>
     <t>Done</t>
@@ -866,13 +863,13 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>12</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2179,7 +2176,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2297,7 +2294,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -2333,7 +2330,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -2371,7 +2368,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -2386,12 +2383,14 @@
       </c>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
+      <c r="R7" s="2">
+        <v>1</v>
+      </c>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2">
         <f>E7-SUM(G7:T7)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -2407,7 +2406,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -2420,12 +2419,14 @@
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
+      <c r="R8" s="2">
+        <v>1</v>
+      </c>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -2445,7 +2446,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G9" s="2">
         <v>1</v>
@@ -2483,7 +2484,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -2519,7 +2520,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -2532,12 +2533,14 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
+      <c r="R11" s="2">
+        <v>1</v>
+      </c>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -2553,7 +2556,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -2591,7 +2594,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -2604,12 +2607,14 @@
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
+      <c r="R13" s="2">
+        <v>1</v>
+      </c>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -2673,7 +2678,7 @@
       </c>
       <c r="R14" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S14" s="2">
         <f t="shared" si="1"/>
@@ -2685,7 +2690,7 @@
       </c>
       <c r="U14" s="2">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -2816,15 +2821,15 @@
       </c>
       <c r="R16" s="2">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="S16" s="2">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="T16" s="2">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="U16" s="11"/>
     </row>

</xml_diff>

<commit_message>
Sprint2 planning and closing Sprint1
</commit_message>
<xml_diff>
--- a/Sprint_info/Sprint1.xlsx
+++ b/Sprint_info/Sprint1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -173,9 +173,6 @@
   </si>
   <si>
     <t>Done</t>
-  </si>
-  <si>
-    <t>In progress</t>
   </si>
 </sst>
 </file>
@@ -869,7 +866,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2176,7 +2173,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2406,7 +2403,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -2423,10 +2420,12 @@
         <v>1</v>
       </c>
       <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
+      <c r="T8" s="2">
+        <v>2</v>
+      </c>
       <c r="U8" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -2520,7 +2519,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -2537,10 +2536,12 @@
         <v>1</v>
       </c>
       <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
+      <c r="T11" s="2">
+        <v>4</v>
+      </c>
       <c r="U11" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -2594,7 +2595,7 @@
         <v>3</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -2611,10 +2612,12 @@
         <v>1</v>
       </c>
       <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
+      <c r="T13" s="2">
+        <v>2</v>
+      </c>
       <c r="U13" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -2686,11 +2689,11 @@
       </c>
       <c r="T14" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U14" s="2">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -2829,7 +2832,7 @@
       </c>
       <c r="T16" s="2">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="U16" s="11"/>
     </row>

</xml_diff>